<commit_message>
Finish PAP and BOM
</commit_message>
<xml_diff>
--- a/PCB-RevA/BOM/BOM-JLCPCB.xlsx
+++ b/PCB-RevA/BOM/BOM-JLCPCB.xlsx
@@ -421,7 +421,7 @@
     <t xml:space="preserve">https://www.lcsc.com/product-detail/Chip-Resistor-Surface-Mount_UNI-ROYAL-Uniroyal-Elec-0402WGF2203TCE_C25767.html</t>
   </si>
   <si>
-    <t xml:space="preserve">R58, R76, R77, R82, R83, R98, R99, R102, R103, R106, R108, R117, R119, R126, R127, R132, R133, R148, R149, R154, R167, R169, R174, R175, R180, R181, R186, R187, R188, R189, R194, R195, R200, R201, R209, R210, R215, R216, R221-R224, R229, R230, R235, R236</t>
+    <t xml:space="preserve">R58, R76, R77, R82, R83, R98, R99, R102, R103, R106, R108, R117, R119, R126, R127, R132, R133, R148, R149, R154, R167, R169, R174, R175, R180, R181, R186, R187, R188, R189, R194, R195, R200, R201, R209, R210, R215, R216, R221, R222, R223, R224, R229, R230, R235, R236</t>
   </si>
   <si>
     <t xml:space="preserve">100K</t>
@@ -490,10 +490,10 @@
     <t xml:space="preserve">Button_Switch_SMD:SW_Push_1P1T_NO_6x6mm_H9.5mm</t>
   </si>
   <si>
-    <t xml:space="preserve">C963229 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.lcsc.com/product-detail/Tactile-Switches_G-Switch-GT-TC074E-H080-L1_C963229.html</t>
+    <t xml:space="preserve">C255812 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.lcsc.com/product-detail/Tactile-Switches_HYP-Hongyuan-Precision-1TS005F-2500-5001_C255812.html</t>
   </si>
   <si>
     <t xml:space="preserve">U1</t>
@@ -535,10 +535,10 @@
     <t xml:space="preserve">Package_SO:SOIC-8_5.275x5.275mm_P1.27mm</t>
   </si>
   <si>
-    <t xml:space="preserve">C115407 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.lcsc.com/product-detail/NOR-FLASH_Winbond-Elec-W25Q16JVSNIQ_C115407.html</t>
+    <t xml:space="preserve">C82317 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.lcsc.com/product-detail/NOR-FLASH_Winbond-Elec-W25Q16JVSSIQ_C82317.html</t>
   </si>
   <si>
     <t xml:space="preserve">U5</t>
@@ -622,10 +622,10 @@
     <t xml:space="preserve">SN74LVC1G14DBV</t>
   </si>
   <si>
-    <t xml:space="preserve">C2976657 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.lcsc.com/product-detail/Gates_UMW-Youtai-Semiconductor-Co-Ltd-SN74LVC1G14DCKR_C2976657.html</t>
+    <t xml:space="preserve">C434069 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.lcsc.com/product-detail/Inverters_UMW-Youtai-Semiconductor-Co-Ltd-SN74LVC1G14DBVR_C434069.html</t>
   </si>
   <si>
     <t xml:space="preserve">U17, U23</t>
@@ -861,11 +861,11 @@
   </sheetPr>
   <dimension ref="A1:P50"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D10" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F25" activeCellId="0" sqref="F25"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A32" activeCellId="0" sqref="A32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.72265625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="35.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="37.57"/>
@@ -2024,7 +2024,7 @@
       <c r="D39" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="E39" s="3" t="s">
+      <c r="E39" s="4" t="s">
         <v>171</v>
       </c>
       <c r="F39" s="1" t="s">
@@ -2204,7 +2204,7 @@
       <c r="D45" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="E45" s="3" t="s">
+      <c r="E45" s="4" t="s">
         <v>200</v>
       </c>
       <c r="F45" s="1" t="s">
@@ -2336,6 +2336,9 @@
       <c r="P50" s="1"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E39" r:id="rId1" display="C82317 "/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>